<commit_message>
fix current_week and check elimination call
</commit_message>
<xml_diff>
--- a/data/playerlist.xlsx
+++ b/data/playerlist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryan\.vscode\Project\FootballDeathPool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0BBC0E-11C8-40C3-B212-8C3DF2BB207C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3B102D-983F-4594-B025-577DC92008A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28890" yWindow="0" windowWidth="28485" windowHeight="14415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="315" yWindow="1785" windowWidth="28485" windowHeight="14415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Death Pool" sheetId="1" r:id="rId1"/>
@@ -86,15 +86,9 @@
     <t>Eagles</t>
   </si>
   <si>
-    <t>Bengles</t>
-  </si>
-  <si>
     <t>Chiefs</t>
   </si>
   <si>
-    <t xml:space="preserve">Seahawks </t>
-  </si>
-  <si>
     <t>Week2</t>
   </si>
   <si>
@@ -171,6 +165,12 @@
   </si>
   <si>
     <t>Active</t>
+  </si>
+  <si>
+    <t>Bengals</t>
+  </si>
+  <si>
+    <t>Seahawks</t>
   </si>
 </sst>
 </file>
@@ -562,7 +562,7 @@
   <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,61 +577,61 @@
         <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -639,13 +639,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -653,13 +653,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -667,13 +667,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -681,7 +681,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>
@@ -695,13 +695,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -709,13 +709,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -723,10 +723,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>15</v>
@@ -737,13 +737,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -751,13 +751,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -765,13 +765,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -779,13 +779,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -793,13 +793,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added debug for check_elimination func
</commit_message>
<xml_diff>
--- a/data/playerlist.xlsx
+++ b/data/playerlist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryan\.vscode\Project\FootballDeathPool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3B102D-983F-4594-B025-577DC92008A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B67E93-B4BC-4475-9688-59EF209F4A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="1785" windowWidth="28485" windowHeight="14415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="1050" windowWidth="28485" windowHeight="14415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Death Pool" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
   <si>
     <t>Jim</t>
   </si>
@@ -171,6 +171,15 @@
   </si>
   <si>
     <t>Seahawks</t>
+  </si>
+  <si>
+    <t>Dolphins</t>
+  </si>
+  <si>
+    <t>Packers</t>
+  </si>
+  <si>
+    <t>Jaguars</t>
   </si>
 </sst>
 </file>
@@ -562,7 +571,7 @@
   <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,6 +656,9 @@
       <c r="D2" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -661,6 +673,9 @@
       <c r="D3" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -689,6 +704,9 @@
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -717,6 +735,9 @@
       <c r="D7" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -731,6 +752,9 @@
       <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -745,6 +769,9 @@
       <c r="D9" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -758,6 +785,9 @@
       </c>
       <c r="D10" s="5" t="s">
         <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update playerlist df eliminated
</commit_message>
<xml_diff>
--- a/data/playerlist.xlsx
+++ b/data/playerlist.xlsx
@@ -745,7 +745,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Eliminated</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -787,7 +787,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Eliminated</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -871,7 +871,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Eliminated</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">

</xml_diff>